<commit_message>
fix past and planned retire code
</commit_message>
<xml_diff>
--- a/data_wrangling_2/raw_data/planned_retire_groupings.xlsx
+++ b/data_wrangling_2/raw_data/planned_retire_groupings.xlsx
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1.494</v>
+        <v>1.528</v>
       </c>
     </row>
     <row r="11">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6.098</v>
+        <v>6.064</v>
       </c>
     </row>
     <row r="14">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1429.6134</v>
+        <v>1430.5294</v>
       </c>
     </row>
     <row r="19">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20.607</v>
+        <v>19.691</v>
       </c>
     </row>
     <row r="22">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.67</v>
+        <v>1.77</v>
       </c>
     </row>
     <row r="35">
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.42</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="38">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.35</v>
+        <v>0.426</v>
       </c>
     </row>
     <row r="43">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.824</v>
       </c>
     </row>
     <row r="46">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="59">
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>3.2708</v>
+        <v>2.9708</v>
       </c>
     </row>
     <row r="62">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>0.334</v>
       </c>
     </row>
     <row r="63">
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.166</v>
+        <v>1.832</v>
       </c>
     </row>
     <row r="66">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1145.846</v>
+        <v>1146.536</v>
       </c>
     </row>
     <row r="67">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>3.95</v>
+        <v>3.26</v>
       </c>
     </row>
     <row r="70">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>0.7869999999999999</v>
       </c>
     </row>
     <row r="91">
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1.198</v>
+        <v>0.411</v>
       </c>
     </row>
     <row r="94">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>31.3989</v>
+        <v>36.5322</v>
       </c>
     </row>
     <row r="103">
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>51.6429</v>
+        <v>46.5096</v>
       </c>
     </row>
     <row r="106">
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0</v>
+        <v>0.122</v>
       </c>
     </row>
     <row r="127">
@@ -2367,7 +2367,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>2.029</v>
+        <v>1.907</v>
       </c>
     </row>
     <row r="130">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1673.5166</v>
+        <v>1686.7424</v>
       </c>
     </row>
     <row r="131">
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>177.0753</v>
+        <v>163.8495</v>
       </c>
     </row>
     <row r="134">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>135.7235</v>
+        <v>144.307</v>
       </c>
     </row>
     <row r="135">
@@ -2487,7 +2487,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>113.9719</v>
+        <v>105.3884</v>
       </c>
     </row>
     <row r="138">
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>7.603</v>
+        <v>9.83</v>
       </c>
     </row>
     <row r="143">
@@ -2607,7 +2607,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>18.6635</v>
+        <v>16.4365</v>
       </c>
     </row>
     <row r="146">
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1809.3715</v>
+        <v>1823.5223</v>
       </c>
     </row>
     <row r="151">
@@ -2727,7 +2727,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>201.6663</v>
+        <v>187.5155</v>
       </c>
     </row>
     <row r="154">
@@ -3102,7 +3102,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>0.13</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="179">
@@ -3147,7 +3147,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>1.004</v>
+        <v>0.884</v>
       </c>
     </row>
     <row r="182">
@@ -3222,7 +3222,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>49.8876</v>
+        <v>50.0116</v>
       </c>
     </row>
     <row r="187">
@@ -3267,7 +3267,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.319</v>
+        <v>0.195</v>
       </c>
     </row>
     <row r="190">
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>0</v>
+        <v>0.336</v>
       </c>
     </row>
     <row r="203">
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>6.166</v>
+        <v>5.83</v>
       </c>
     </row>
     <row r="206">
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>50.6332</v>
+        <v>51.7432</v>
       </c>
     </row>
     <row r="211">
@@ -3627,7 +3627,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>2.5268</v>
+        <v>1.4168</v>
       </c>
     </row>
     <row r="214">
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>12.333</v>
+        <v>12.433</v>
       </c>
     </row>
     <row r="215">
@@ -3687,7 +3687,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>1.273</v>
+        <v>1.173</v>
       </c>
     </row>
     <row r="218">
@@ -5142,7 +5142,7 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>189.4546</v>
+        <v>201.6404</v>
       </c>
     </row>
     <row r="315">
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>157.5803</v>
+        <v>145.3945</v>
       </c>
     </row>
     <row r="318">
@@ -5562,7 +5562,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>10.4371</v>
+        <v>11.1691</v>
       </c>
     </row>
     <row r="343">
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>8.212899999999999</v>
+        <v>7.4809</v>
       </c>
     </row>
     <row r="346">
@@ -5742,7 +5742,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>33.6361</v>
+        <v>33.7861</v>
       </c>
     </row>
     <row r="355">
@@ -5787,7 +5787,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>4.175</v>
+        <v>4.025</v>
       </c>
     </row>
     <row r="358">
@@ -5862,7 +5862,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>3.346</v>
+        <v>3.737</v>
       </c>
     </row>
     <row r="363">
@@ -5907,7 +5907,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>1.121</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="366">
@@ -5982,7 +5982,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>0.05</v>
+        <v>0.124</v>
       </c>
     </row>
     <row r="371">
@@ -6027,7 +6027,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>0.07400000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="374">
@@ -6102,7 +6102,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>8.481</v>
+        <v>9.601000000000001</v>
       </c>
     </row>
     <row r="379">
@@ -6147,7 +6147,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>9.52</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="382">
@@ -6162,7 +6162,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>1.299</v>
+        <v>2.0343</v>
       </c>
     </row>
     <row r="383">
@@ -6207,7 +6207,7 @@
         </is>
       </c>
       <c r="C385" t="n">
-        <v>1.6015</v>
+        <v>0.8662000000000001</v>
       </c>
     </row>
     <row r="386">
@@ -6882,7 +6882,7 @@
         </is>
       </c>
       <c r="C430" t="n">
-        <v>0</v>
+        <v>2.172</v>
       </c>
     </row>
     <row r="431">
@@ -6927,7 +6927,7 @@
         </is>
       </c>
       <c r="C433" t="n">
-        <v>2.172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="434">
@@ -6942,7 +6942,7 @@
         </is>
       </c>
       <c r="C434" t="n">
-        <v>77.4873</v>
+        <v>79.8038</v>
       </c>
     </row>
     <row r="435">
@@ -6987,7 +6987,7 @@
         </is>
       </c>
       <c r="C437" t="n">
-        <v>79.1438</v>
+        <v>76.82729999999999</v>
       </c>
     </row>
     <row r="438">

</xml_diff>

<commit_message>
squashing 9 commits to get this to push to heroku
Update README.md

update title

fix retire groupings

fix missing 2050 data

fix capacity over time df

fresh start package-lock

updated package.json

added glob-parent@6.0.2

Create app.json to use heroku 22
</commit_message>
<xml_diff>
--- a/data_wrangling_2/raw_data/planned_retire_groupings.xlsx
+++ b/data_wrangling_2/raw_data/planned_retire_groupings.xlsx
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>3.236</v>
       </c>
     </row>
     <row r="12">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>6.495</v>
       </c>
     </row>
     <row r="20">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>0.345</v>
       </c>
     </row>
     <row r="44">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="60">
@@ -1977,7 +1977,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>3.068</v>
       </c>
     </row>
     <row r="104">
@@ -2397,7 +2397,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0</v>
+        <v>30.0296</v>
       </c>
     </row>
     <row r="132">
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0</v>
+        <v>3.9876</v>
       </c>
     </row>
     <row r="136">
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0</v>
+        <v>33.3296</v>
       </c>
     </row>
     <row r="152">
@@ -3237,7 +3237,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="188">
@@ -4137,7 +4137,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248">
@@ -5157,7 +5157,7 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>0</v>
+        <v>23.1346</v>
       </c>
     </row>
     <row r="316">
@@ -5577,7 +5577,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>0</v>
+        <v>3.068</v>
       </c>
     </row>
     <row r="344">
@@ -6057,7 +6057,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>0</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="376">
@@ -6117,7 +6117,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>0</v>
+        <v>12.843</v>
       </c>
     </row>
     <row r="380">
@@ -6237,7 +6237,7 @@
         </is>
       </c>
       <c r="C387" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="388">
@@ -6957,7 +6957,7 @@
         </is>
       </c>
       <c r="C435" t="n">
-        <v>0</v>
+        <v>3.8776</v>
       </c>
     </row>
     <row r="436">

</xml_diff>